<commit_message>
account for timezone more robustly and produce consistent output csv formating
</commit_message>
<xml_diff>
--- a/inst/extdata/S285_ctd.xlsx
+++ b/inst/extdata/S285_ctd.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="30">
   <si>
     <t>S285-002</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>afm_volt_out</t>
-  </si>
-  <si>
-    <t>352</t>
   </si>
   <si>
     <t>volt5</t>
@@ -118,7 +115,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -127,9 +124,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -152,18 +154,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,548 +507,558 @@
   <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="5"/>
+    <col min="2" max="2" width="13.33203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="4"/>
+    <col min="4" max="4" width="14.5" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="4"/>
+    <col min="6" max="11" width="20.33203125" style="5" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" style="5"/>
+    <col min="13" max="13" width="11.5" style="5" customWidth="1"/>
+    <col min="14" max="14" width="12" style="5" customWidth="1"/>
+    <col min="15" max="15" width="11.83203125" style="5" customWidth="1"/>
+    <col min="16" max="16" width="12" style="5" customWidth="1"/>
+    <col min="17" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:16" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" s="4" t="s">
+      <c r="K1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="4">
         <v>910</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="4">
         <v>450</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="4">
         <v>483</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="4">
         <v>389</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="J2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L2" s="5">
         <v>7706</v>
       </c>
-      <c r="M2" s="1">
+      <c r="M2" s="5">
         <v>13.7</v>
       </c>
-      <c r="N2" s="1">
+      <c r="N2" s="5">
         <v>13.5</v>
       </c>
-      <c r="O2" s="1">
+      <c r="O2" s="5">
         <v>11.45</v>
       </c>
-      <c r="P2" s="1">
+      <c r="P2" s="5">
         <v>11.62</v>
       </c>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="4">
         <v>375</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="4">
         <v>412</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="E3" s="4">
+        <v>352</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="J3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="1">
+      <c r="L3" s="5">
         <v>7706</v>
       </c>
-      <c r="M3" s="1">
+      <c r="M3" s="5">
         <v>13.5</v>
       </c>
-      <c r="O3" s="1">
+      <c r="O3" s="5">
         <v>11.45</v>
       </c>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="4">
         <v>900</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
         <v>499</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="4">
         <v>540</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="4">
         <v>490</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" s="1" t="s">
+      <c r="J4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4" s="5">
         <v>7706</v>
       </c>
-      <c r="M4" s="1">
+      <c r="M4" s="5">
         <v>13.3</v>
       </c>
-      <c r="N4" s="1">
+      <c r="N4" s="5">
         <v>13.1</v>
       </c>
-      <c r="O4" s="1">
+      <c r="O4" s="5">
         <v>11.28</v>
       </c>
-      <c r="P4" s="1">
+      <c r="P4" s="5">
         <v>11.3</v>
       </c>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="4">
         <v>595</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="4">
         <v>400</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="4">
         <v>463</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="4">
         <v>391</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" s="1" t="s">
+      <c r="J5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L5" s="5">
         <v>7706</v>
       </c>
-      <c r="M5" s="1">
+      <c r="M5" s="5">
         <v>13.1</v>
       </c>
-      <c r="N5" s="1">
-        <v>13</v>
-      </c>
-      <c r="O5" s="1">
+      <c r="N5" s="5">
+        <v>13</v>
+      </c>
+      <c r="O5" s="5">
         <v>11.2</v>
       </c>
-      <c r="P5" s="1">
+      <c r="P5" s="5">
         <v>11.21</v>
       </c>
     </row>
     <row r="6" spans="1:16">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="4">
         <v>585</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="4">
         <v>400</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="4">
         <v>481</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="4">
         <v>385</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" s="1" t="s">
+      <c r="J6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="1">
+      <c r="L6" s="5">
         <v>7706</v>
       </c>
-      <c r="M6" s="1">
+      <c r="M6" s="5">
         <v>13.1</v>
       </c>
-      <c r="N6" s="1">
-        <v>13</v>
-      </c>
-      <c r="O6" s="1">
+      <c r="N6" s="5">
+        <v>13</v>
+      </c>
+      <c r="O6" s="5">
         <v>12.71</v>
       </c>
-      <c r="P6" s="1">
+      <c r="P6" s="5">
         <v>12.75</v>
       </c>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="4">
         <v>1137</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="4">
         <v>1000</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="4">
         <v>4208</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7" s="1" t="s">
+      <c r="J7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7" s="5">
         <v>7706</v>
       </c>
-      <c r="M7" s="1">
+      <c r="M7" s="5">
         <v>12.9</v>
       </c>
-      <c r="N7" s="1">
-        <v>13</v>
-      </c>
-      <c r="O7" s="1">
+      <c r="N7" s="5">
+        <v>13</v>
+      </c>
+      <c r="O7" s="5">
         <v>12.59</v>
       </c>
-      <c r="P7" s="1">
+      <c r="P7" s="5">
         <v>12.18</v>
       </c>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="4">
         <v>982</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="4">
         <v>300</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="4">
         <v>3932</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="4">
         <v>291</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K8" s="1" t="s">
+      <c r="J8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L8" s="5">
         <v>7706</v>
       </c>
-      <c r="M8" s="1">
-        <v>13</v>
-      </c>
-      <c r="N8" s="1">
-        <v>13</v>
-      </c>
-      <c r="O8" s="1">
+      <c r="M8" s="5">
+        <v>13</v>
+      </c>
+      <c r="N8" s="5">
+        <v>13</v>
+      </c>
+      <c r="O8" s="5">
         <v>12</v>
       </c>
-      <c r="P8" s="1">
+      <c r="P8" s="5">
         <v>12.11</v>
       </c>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="4">
         <v>1100</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="4">
         <v>4536</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="4">
         <v>916</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K9" s="1" t="s">
+      <c r="J9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9" s="5">
         <v>7706</v>
       </c>
-      <c r="M9" s="1">
+      <c r="M9" s="5">
         <v>12.8</v>
       </c>
-      <c r="N9" s="1">
+      <c r="N9" s="5">
         <v>12.5</v>
       </c>
-      <c r="O9" s="1">
+      <c r="O9" s="5">
         <v>12.06</v>
       </c>
-      <c r="P9" s="1">
+      <c r="P9" s="5">
         <v>11.87</v>
       </c>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="4">
         <v>1057</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="4">
         <v>1200</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="4">
         <v>4829</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="4">
         <v>914</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K10" s="1" t="s">
+      <c r="J10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L10" s="1">
+      <c r="L10" s="5">
         <v>7706</v>
       </c>
-      <c r="M10" s="1">
+      <c r="M10" s="5">
         <v>12.7</v>
       </c>
-      <c r="N10" s="1">
+      <c r="N10" s="5">
         <v>12.4</v>
       </c>
-      <c r="O10" s="1">
+      <c r="O10" s="5">
         <v>11.84</v>
       </c>
-      <c r="P10" s="1">
+      <c r="P10" s="5">
         <v>11.62</v>
       </c>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="4">
         <v>400</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="4">
         <v>5187</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="4">
         <v>386</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K11" s="1" t="s">
+      <c r="J11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L11" s="1">
+      <c r="L11" s="5">
         <v>7706</v>
       </c>
-      <c r="M11" s="1">
+      <c r="M11" s="5">
         <v>12.5</v>
       </c>
-      <c r="N11" s="1">
+      <c r="N11" s="5">
         <v>12.4</v>
       </c>
-      <c r="O11" s="1">
+      <c r="O11" s="5">
         <v>11.66</v>
       </c>
-      <c r="P11" s="1">
+      <c r="P11" s="5">
         <v>11.6</v>
       </c>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" s="2"/>
+      <c r="A12" s="3"/>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" s="2"/>
+      <c r="A13" s="3"/>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="2"/>
+      <c r="A14" s="3"/>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="2"/>
+      <c r="A15" s="3"/>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="2"/>
+      <c r="A16" s="3"/>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="2"/>
+      <c r="A17" s="3"/>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="2"/>
+      <c r="A18" s="3"/>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="2"/>
+      <c r="A19" s="3"/>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="2"/>
+      <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="2"/>
+      <c r="A21" s="3"/>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="2"/>
+      <c r="A22" s="3"/>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="2"/>
+      <c r="A23" s="3"/>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="3"/>
+      <c r="A24" s="6"/>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="3"/>
+      <c r="A25" s="6"/>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="3"/>
+      <c r="A26" s="6"/>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="3"/>
+      <c r="A27" s="6"/>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="3"/>
+      <c r="A28" s="6"/>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="3"/>
+      <c r="A29" s="6"/>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="3"/>
+      <c r="A30" s="6"/>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="3"/>
+      <c r="A31" s="6"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>